<commit_message>
Minor Fixes and Adjustments
</commit_message>
<xml_diff>
--- a/MT.xlsx
+++ b/MT.xlsx
@@ -76,7 +76,10 @@
     <t xml:space="preserve">*</t>
   </si>
   <si>
-    <t xml:space="preserve">IIII</t>
+    <t xml:space="preserve">IIII*III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">L</t>
@@ -86,9 +89,6 @@
   </si>
   <si>
     <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
   </si>
   <si>
     <t xml:space="preserve">H</t>
@@ -339,10 +339,10 @@
   <dimension ref="B1:N35"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="11" style="0" width="20.41"/>
@@ -401,7 +401,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F4" s="7" t="n">
         <v>0</v>
@@ -413,7 +413,7 @@
         <v>10</v>
       </c>
       <c r="I4" s="7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="4" t="n">
         <v>0</v>
@@ -422,7 +422,7 @@
         <v>8</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N4" s="4" t="n">
         <v>0</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -438,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>10</v>
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N5" s="4" t="n">
         <v>1</v>
@@ -465,11 +465,11 @@
       </c>
       <c r="C6" s="4" t="str">
         <f aca="false">_xlfn.CONCAT("1-",LEN(C4))</f>
-        <v>1-4</v>
+        <v>1-8</v>
       </c>
       <c r="D6" s="4" t="n">
         <f aca="false">LEN(C4)+1</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F6" s="7" t="n">
         <v>1</v>
@@ -478,7 +478,7 @@
         <v>8</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I6" s="7" t="n">
         <v>2</v>
@@ -490,7 +490,7 @@
         <v>8</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N6" s="4" t="n">
         <v>2</v>
@@ -501,7 +501,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>10</v>
@@ -513,10 +513,10 @@
         <v>1</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N7" s="4" t="n">
         <v>1</v>
@@ -530,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I8" s="7" t="n">
         <v>3</v>
@@ -555,10 +555,10 @@
         <v>2</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I9" s="7" t="n">
         <v>2</v>
@@ -567,10 +567,10 @@
         <v>2</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N9" s="4" t="n">
         <v>3</v>
@@ -584,7 +584,7 @@
         <v>8</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I10" s="7" t="n">
         <v>4</v>
@@ -607,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>8</v>
@@ -619,10 +619,10 @@
         <v>3</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N11" s="4" t="n">
         <v>3</v>
@@ -651,7 +651,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H13" s="4" t="s">
         <v>8</v>
@@ -678,7 +678,7 @@
         <v>8</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N14" s="7" t="n">
         <v>1</v>
@@ -693,10 +693,10 @@
         <v>0</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N15" s="7" t="n">
         <v>1</v>
@@ -714,7 +714,7 @@
         <v>8</v>
       </c>
       <c r="M16" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N16" s="7" t="n">
         <v>2</v>
@@ -725,10 +725,10 @@
         <v>1</v>
       </c>
       <c r="L17" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M17" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N17" s="7" t="n">
         <v>1</v>
@@ -742,7 +742,7 @@
         <v>8</v>
       </c>
       <c r="M18" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N18" s="7" t="n">
         <v>3</v>
@@ -753,10 +753,10 @@
         <v>2</v>
       </c>
       <c r="L19" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M19" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N19" s="7" t="n">
         <v>2</v>
@@ -770,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N20" s="7" t="n">
         <v>4</v>
@@ -781,7 +781,7 @@
         <v>3</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M21" s="7" t="s">
         <v>8</v>
@@ -809,7 +809,7 @@
         <v>4</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M23" s="4" t="s">
         <v>8</v>
@@ -834,7 +834,7 @@
         <v>8</v>
       </c>
       <c r="M26" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N26" s="7" t="n">
         <v>0</v>
@@ -845,10 +845,10 @@
         <v>0</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N27" s="7" t="n">
         <v>1</v>
@@ -862,7 +862,7 @@
         <v>8</v>
       </c>
       <c r="M28" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="N28" s="7" t="n">
         <v>2</v>
@@ -873,10 +873,10 @@
         <v>1</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M29" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N29" s="7" t="n">
         <v>1</v>
@@ -890,7 +890,7 @@
         <v>8</v>
       </c>
       <c r="M30" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N30" s="7" t="n">
         <v>3</v>
@@ -901,10 +901,10 @@
         <v>2</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="N31" s="7" t="n">
         <v>2</v>
@@ -918,7 +918,7 @@
         <v>8</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N32" s="7" t="n">
         <v>4</v>
@@ -929,7 +929,7 @@
         <v>3</v>
       </c>
       <c r="L33" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M33" s="7" t="s">
         <v>8</v>
@@ -957,7 +957,7 @@
         <v>4</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="M35" s="4" t="s">
         <v>8</v>

</xml_diff>